<commit_message>
Make small updates to ensure continued operability of processes.
</commit_message>
<xml_diff>
--- a/Finding_City_Weather/city_weather.xlsx
+++ b/Finding_City_Weather/city_weather.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <x:si>
     <x:t>Current TimeStamp</x:t>
   </x:si>
@@ -41,94 +41,73 @@
     <x:t>Wind Speed</x:t>
   </x:si>
   <x:si>
-    <x:t>12/17/2021 10:59:35</x:t>
+    <x:t>12/29/2022 10:46:49</x:t>
   </x:si>
   <x:si>
     <x:t>Kansas City</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>59%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/17/2021 10:59:37</x:t>
+    <x:t>63</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/29/2022 10:46:52</x:t>
   </x:si>
   <x:si>
     <x:t>New York</x:t>
   </x:si>
   <x:si>
-    <x:t>58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/17/2021 10:59:39</x:t>
+    <x:t>44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/29/2022 10:46:55</x:t>
   </x:si>
   <x:si>
     <x:t>Sacramento</x:t>
   </x:si>
   <x:si>
-    <x:t>39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>96%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/17/2021 10:59:42</x:t>
+    <x:t>40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>85%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/29/2022 10:46:58</x:t>
   </x:si>
   <x:si>
     <x:t>Chicago</x:t>
   </x:si>
   <x:si>
-    <x:t>36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>54%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/17/2021 10:59:44</x:t>
+    <x:t>52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/29/2022 10:47:00</x:t>
   </x:si>
   <x:si>
     <x:t>Nashville</x:t>
   </x:si>
   <x:si>
-    <x:t>56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>89%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 mph</x:t>
+    <x:t>60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 mph</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -526,87 +505,87 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F2" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B3" s="2" t="s">
+      <x:c r="C3" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="D3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E3" s="2" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="F3" s="2" t="s">
-        <x:v>17</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B4" s="2" t="s">
+      <x:c r="E4" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D4" s="2" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E4" s="2" t="s">
-        <x:v>22</x:v>
-      </x:c>
       <x:c r="F4" s="2" t="s">
-        <x:v>23</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="2" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C5" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
-        <x:v>27</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
-        <x:v>28</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F5" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="2" t="s">
-        <x:v>30</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
-        <x:v>31</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D6" s="2" t="s">
-        <x:v>33</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E6" s="2" t="s">
-        <x:v>34</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F6" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Make change to Finding_City_Weather selector.
</commit_message>
<xml_diff>
--- a/Finding_City_Weather/city_weather.xlsx
+++ b/Finding_City_Weather/city_weather.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <x:si>
     <x:t>Current TimeStamp</x:t>
   </x:si>
@@ -41,73 +41,67 @@
     <x:t>Wind Speed</x:t>
   </x:si>
   <x:si>
-    <x:t>12/29/2022 10:46:49</x:t>
+    <x:t>02/03/2023 12:12:39</x:t>
   </x:si>
   <x:si>
     <x:t>Kansas City</x:t>
   </x:si>
   <x:si>
-    <x:t>63</x:t>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>02/03/2023 12:12:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New York</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>02/03/2023 12:12:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sacramento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>02/03/2023 12:12:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chicago</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
   </x:si>
   <x:si>
     <x:t>1%</x:t>
   </x:si>
   <x:si>
-    <x:t>19 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/29/2022 10:46:52</x:t>
-  </x:si>
-  <x:si>
-    <x:t>New York</x:t>
-  </x:si>
-  <x:si>
-    <x:t>44</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/29/2022 10:46:55</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sacramento</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>85%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/29/2022 10:46:58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chicago</x:t>
-  </x:si>
-  <x:si>
-    <x:t>52</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/29/2022 10:47:00</x:t>
+    <x:t>02/03/2023 12:12:50</x:t>
   </x:si>
   <x:si>
     <x:t>Nashville</x:t>
   </x:si>
   <x:si>
-    <x:t>60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>60%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16 mph</x:t>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9 mph</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -505,27 +499,27 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F2" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C3" s="2" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D3" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F3" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -542,50 +536,50 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="E4" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F4" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B5" s="2" t="s">
+      <x:c r="C5" s="2" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="s">
+      <x:c r="D5" s="2" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="D5" s="2" t="s">
-        <x:v>23</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F5" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B6" s="2" t="s">
+      <x:c r="C6" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C6" s="2" t="s">
+      <x:c r="D6" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="D6" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="E6" s="2" t="s">
-        <x:v>28</x:v>
-      </x:c>
       <x:c r="F6" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>